<commit_message>
Updates BOM for motor power control
</commit_message>
<xml_diff>
--- a/Electrical/PowerControlModule/BOM-PowerControlModule.xlsx
+++ b/Electrical/PowerControlModule/BOM-PowerControlModule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jklei\Desktop\Projects\igvc_hardware_2020\Electrical\PowerControlModule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DF1152E-76A6-4D81-BCB0-41EFD53249B1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A60E528-4582-4D4E-8D36-9AF446F6AC41}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{883824F6-74A7-4AC8-B3B1-99107F04C8A5}"/>
+    <workbookView xWindow="2442" yWindow="2442" windowWidth="17280" windowHeight="8994" xr2:uid="{883824F6-74A7-4AC8-B3B1-99107F04C8A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>Unit Cost</t>
   </si>
@@ -82,6 +82,18 @@
   </si>
   <si>
     <t xml:space="preserve">178.6164.0002 </t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/CUI/HSE-B20250-040H?qs=sGAEpiMZZMttgyDkZ5Wiut%252B4GcHIZ2pKOgousR6bMSo%3D</t>
+  </si>
+  <si>
+    <t>Heatshrink</t>
+  </si>
+  <si>
+    <t>CUI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HSE-B20250-040H </t>
   </si>
 </sst>
 </file>
@@ -473,10 +485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BDFDD80-2A02-4280-B66A-7146443800A2}">
-  <dimension ref="B2:H5"/>
+  <dimension ref="B2:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B2" sqref="B2:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -582,6 +594,30 @@
         <v>13</v>
       </c>
     </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6" s="4">
+        <f>F6*E6</f>
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="H6" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H4" r:id="rId1" xr:uid="{B0523331-2142-4164-A167-57F4B5387FCC}"/>

</xml_diff>